<commit_message>
exercitiile de la curs mai explicate + intro arrays
</commit_message>
<xml_diff>
--- a/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
+++ b/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Geoinformatica_Promotia_2025_2028\AlgoritmiSiStructuriDeDate1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20FE2AF-564E-41FB-AD92-3AC3FFDD6641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBA40E7-2283-4E0E-9D41-BB7B97C034D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -673,10 +673,10 @@
   <dimension ref="B2:R52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -750,7 +750,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -765,7 +765,7 @@
       <c r="P3" s="7"/>
       <c r="Q3" s="8">
         <f>SUM(C3:P3)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R3" s="7"/>
     </row>
@@ -811,12 +811,12 @@
         <v>1</v>
       </c>
       <c r="E6" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R6" s="10"/>
     </row>
@@ -848,12 +848,12 @@
         <v>1</v>
       </c>
       <c r="E8" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R8" s="10"/>
     </row>
@@ -928,12 +928,12 @@
         <v>2</v>
       </c>
       <c r="E12" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R12" s="10"/>
     </row>
@@ -945,12 +945,12 @@
         <v>1</v>
       </c>
       <c r="E13" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R13" s="10"/>
     </row>
@@ -965,12 +965,12 @@
         <v>2</v>
       </c>
       <c r="E14" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R14" s="10"/>
     </row>
@@ -1022,12 +1022,12 @@
         <v>2</v>
       </c>
       <c r="E17" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R17" s="10"/>
     </row>
@@ -1042,12 +1042,12 @@
         <v>2</v>
       </c>
       <c r="E18" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R18" s="10"/>
     </row>
@@ -1062,12 +1062,12 @@
         <v>2</v>
       </c>
       <c r="E19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R19" s="10"/>
     </row>
@@ -1102,12 +1102,12 @@
         <v>2</v>
       </c>
       <c r="E21" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R21" s="10"/>
     </row>

</xml_diff>

<commit_message>
structuri, enumeratii, constante; algoritmul pentru verificarea daca un numar este prim
</commit_message>
<xml_diff>
--- a/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
+++ b/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Geoinformatica_Promotia_2025_2028\AlgoritmiSiStructuriDeDate1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBA40E7-2283-4E0E-9D41-BB7B97C034D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A89E6B-1CEF-4F09-BB2F-5242650D3A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -673,7 +673,7 @@
   <dimension ref="B2:R52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
@@ -813,10 +813,13 @@
       <c r="E6" s="3">
         <v>2</v>
       </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R6" s="10"/>
     </row>
@@ -870,10 +873,13 @@
       <c r="E9" s="3">
         <v>1</v>
       </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R9" s="10"/>
     </row>
@@ -890,10 +896,13 @@
       <c r="E10" s="3">
         <v>1</v>
       </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R10" s="10"/>
     </row>
@@ -930,10 +939,13 @@
       <c r="E12" s="3">
         <v>2</v>
       </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R12" s="10"/>
     </row>
@@ -947,10 +959,13 @@
       <c r="E13" s="3">
         <v>2</v>
       </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R13" s="10"/>
     </row>
@@ -967,10 +982,13 @@
       <c r="E14" s="3">
         <v>2</v>
       </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R14" s="10"/>
     </row>
@@ -1024,10 +1042,13 @@
       <c r="E17" s="3">
         <v>2</v>
       </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R17" s="10"/>
     </row>
@@ -1044,10 +1065,13 @@
       <c r="E18" s="3">
         <v>2</v>
       </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R18" s="10"/>
     </row>
@@ -1064,10 +1088,13 @@
       <c r="E19" s="3">
         <v>2</v>
       </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R19" s="10"/>
     </row>
@@ -1104,10 +1131,13 @@
       <c r="E21" s="3">
         <v>2</v>
       </c>
+      <c r="F21" s="3">
+        <v>1</v>
+      </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R21" s="10"/>
     </row>

</xml_diff>

<commit_message>
probleme de la structura decisiva de dificultate medie
</commit_message>
<xml_diff>
--- a/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
+++ b/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Geoinformatica_Promotia_2025_2028\AlgoritmiSiStructuriDeDate1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A89E6B-1CEF-4F09-BB2F-5242650D3A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B14690-1A1B-4D2E-AD94-7215C65F571F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -673,10 +673,10 @@
   <dimension ref="B2:R52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -782,10 +782,13 @@
       <c r="E4" s="3">
         <v>1</v>
       </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
       <c r="P4" s="10"/>
       <c r="Q4" s="8">
         <f t="shared" ref="Q4:Q52" si="0">SUM(C4:P4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R4" s="10"/>
     </row>
@@ -814,12 +817,12 @@
         <v>2</v>
       </c>
       <c r="F6" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R6" s="10"/>
     </row>
@@ -833,10 +836,13 @@
       <c r="D7" s="3">
         <v>1</v>
       </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R7" s="10"/>
     </row>
@@ -853,10 +859,13 @@
       <c r="E8" s="3">
         <v>2</v>
       </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R8" s="10"/>
     </row>
@@ -874,12 +883,12 @@
         <v>1</v>
       </c>
       <c r="F9" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R9" s="10"/>
     </row>
@@ -897,12 +906,12 @@
         <v>1</v>
       </c>
       <c r="F10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R10" s="10"/>
     </row>
@@ -919,10 +928,13 @@
       <c r="E11" s="3">
         <v>1</v>
       </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
       <c r="P11" s="10"/>
       <c r="Q11" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R11" s="10"/>
     </row>
@@ -940,12 +952,12 @@
         <v>2</v>
       </c>
       <c r="F12" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R12" s="10"/>
     </row>
@@ -960,12 +972,12 @@
         <v>2</v>
       </c>
       <c r="F13" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R13" s="10"/>
     </row>
@@ -983,12 +995,12 @@
         <v>2</v>
       </c>
       <c r="F14" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R14" s="10"/>
     </row>
@@ -1022,10 +1034,13 @@
       <c r="E16" s="3">
         <v>1</v>
       </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
       <c r="P16" s="10"/>
       <c r="Q16" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R16" s="10"/>
     </row>
@@ -1043,12 +1058,12 @@
         <v>2</v>
       </c>
       <c r="F17" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R17" s="10"/>
     </row>
@@ -1066,12 +1081,12 @@
         <v>2</v>
       </c>
       <c r="F18" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R18" s="10"/>
     </row>
@@ -1089,12 +1104,12 @@
         <v>2</v>
       </c>
       <c r="F19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R19" s="10"/>
     </row>
@@ -1111,10 +1126,13 @@
       <c r="E20" s="3">
         <v>1</v>
       </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R20" s="10"/>
     </row>
@@ -1132,12 +1150,12 @@
         <v>2</v>
       </c>
       <c r="F21" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R21" s="10"/>
     </row>

</xml_diff>

<commit_message>
operatori, operatori pe biti, operatori diversi, cu explicatii si exemple
</commit_message>
<xml_diff>
--- a/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
+++ b/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Geoinformatica_Promotia_2025_2028\AlgoritmiSiStructuriDeDate1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B14690-1A1B-4D2E-AD94-7215C65F571F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED26E0E-84AB-4C25-800A-25FD71E2F3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -676,7 +676,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -753,7 +753,9 @@
         <v>2</v>
       </c>
       <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -765,7 +767,7 @@
       <c r="P3" s="7"/>
       <c r="Q3" s="8">
         <f>SUM(C3:P3)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R3" s="7"/>
     </row>
@@ -785,10 +787,13 @@
       <c r="F4" s="3">
         <v>1</v>
       </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
       <c r="P4" s="10"/>
       <c r="Q4" s="8">
         <f t="shared" ref="Q4:Q52" si="0">SUM(C4:P4)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R4" s="10"/>
     </row>
@@ -819,10 +824,13 @@
       <c r="F6" s="3">
         <v>2</v>
       </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R6" s="10"/>
     </row>
@@ -839,10 +847,13 @@
       <c r="F7" s="3">
         <v>1</v>
       </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R7" s="10"/>
     </row>
@@ -862,10 +873,13 @@
       <c r="F8" s="3">
         <v>1</v>
       </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R8" s="10"/>
     </row>
@@ -908,10 +922,13 @@
       <c r="F10" s="3">
         <v>2</v>
       </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R10" s="10"/>
     </row>
@@ -931,10 +948,13 @@
       <c r="F11" s="3">
         <v>1</v>
       </c>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
       <c r="P11" s="10"/>
       <c r="Q11" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R11" s="10"/>
     </row>
@@ -954,10 +974,13 @@
       <c r="F12" s="3">
         <v>2</v>
       </c>
+      <c r="G12" s="3">
+        <v>1</v>
+      </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R12" s="10"/>
     </row>
@@ -974,10 +997,13 @@
       <c r="F13" s="3">
         <v>2</v>
       </c>
+      <c r="G13" s="3">
+        <v>1</v>
+      </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R13" s="10"/>
     </row>
@@ -997,10 +1023,13 @@
       <c r="F14" s="3">
         <v>2</v>
       </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R14" s="10"/>
     </row>
@@ -1037,10 +1066,13 @@
       <c r="F16" s="3">
         <v>1</v>
       </c>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
       <c r="P16" s="10"/>
       <c r="Q16" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R16" s="10"/>
     </row>
@@ -1060,10 +1092,13 @@
       <c r="F17" s="3">
         <v>2</v>
       </c>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R17" s="10"/>
     </row>
@@ -1083,10 +1118,13 @@
       <c r="F18" s="3">
         <v>2</v>
       </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R18" s="10"/>
     </row>
@@ -1106,10 +1144,13 @@
       <c r="F19" s="3">
         <v>2</v>
       </c>
+      <c r="G19" s="3">
+        <v>1</v>
+      </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R19" s="10"/>
     </row>
@@ -1129,10 +1170,13 @@
       <c r="F20" s="3">
         <v>1</v>
       </c>
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R20" s="10"/>
     </row>
@@ -1152,10 +1196,13 @@
       <c r="F21" s="3">
         <v>2</v>
       </c>
+      <c r="G21" s="3">
+        <v>1</v>
+      </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R21" s="10"/>
     </row>
@@ -1487,7 +1534,7 @@
   </sortState>
   <conditionalFormatting sqref="Q3:Q52">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
-      <formula>8</formula>
+      <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
structura repetitiva. modul de gandire "2D" cu doua for-uri
</commit_message>
<xml_diff>
--- a/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
+++ b/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Geoinformatica_Promotia_2025_2028\AlgoritmiSiStructuriDeDate1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED26E0E-84AB-4C25-800A-25FD71E2F3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E006909-E378-443C-A100-78EAE6C4AAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -676,7 +676,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -754,7 +754,7 @@
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -767,7 +767,7 @@
       <c r="P3" s="7"/>
       <c r="Q3" s="8">
         <f>SUM(C3:P3)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R3" s="7"/>
     </row>
@@ -825,12 +825,12 @@
         <v>2</v>
       </c>
       <c r="G6" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R6" s="10"/>
     </row>
@@ -848,12 +848,12 @@
         <v>1</v>
       </c>
       <c r="G7" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R7" s="10"/>
     </row>
@@ -899,10 +899,13 @@
       <c r="F9" s="3">
         <v>2</v>
       </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R9" s="10"/>
     </row>
@@ -975,12 +978,12 @@
         <v>2</v>
       </c>
       <c r="G12" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="8">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R12" s="10"/>
     </row>
@@ -998,12 +1001,12 @@
         <v>2</v>
       </c>
       <c r="G13" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R13" s="10"/>
     </row>
@@ -1024,12 +1027,12 @@
         <v>2</v>
       </c>
       <c r="G14" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="8">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R14" s="10"/>
     </row>
@@ -1093,12 +1096,12 @@
         <v>2</v>
       </c>
       <c r="G17" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R17" s="10"/>
     </row>
@@ -1119,12 +1122,12 @@
         <v>2</v>
       </c>
       <c r="G18" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="8">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R18" s="10"/>
     </row>
@@ -1145,12 +1148,12 @@
         <v>2</v>
       </c>
       <c r="G19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="8">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R19" s="10"/>
     </row>
@@ -1197,12 +1200,12 @@
         <v>2</v>
       </c>
       <c r="G21" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R21" s="10"/>
     </row>

</xml_diff>

<commit_message>
structura de decizie si structura switch
</commit_message>
<xml_diff>
--- a/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
+++ b/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Geoinformatica_Promotia_2025_2028\AlgoritmiSiStructuriDeDate1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E006909-E378-443C-A100-78EAE6C4AAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9E24B7-4B63-475A-8A5B-29295A50BD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -672,11 +672,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -827,10 +827,13 @@
       <c r="G6" s="3">
         <v>2</v>
       </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R6" s="10"/>
     </row>
@@ -902,10 +905,13 @@
       <c r="G9" s="3">
         <v>1</v>
       </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R9" s="10"/>
     </row>
@@ -980,10 +986,13 @@
       <c r="G12" s="3">
         <v>2</v>
       </c>
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="8">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R12" s="10"/>
     </row>
@@ -1003,10 +1012,13 @@
       <c r="G13" s="3">
         <v>2</v>
       </c>
+      <c r="H13" s="3">
+        <v>1</v>
+      </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R13" s="10"/>
     </row>
@@ -1029,10 +1041,13 @@
       <c r="G14" s="3">
         <v>2</v>
       </c>
+      <c r="H14" s="3">
+        <v>1</v>
+      </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="8">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R14" s="10"/>
     </row>
@@ -1124,10 +1139,13 @@
       <c r="G18" s="3">
         <v>2</v>
       </c>
+      <c r="H18" s="3">
+        <v>1</v>
+      </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="8">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R18" s="10"/>
     </row>
@@ -1150,10 +1168,13 @@
       <c r="G19" s="3">
         <v>2</v>
       </c>
+      <c r="H19" s="3">
+        <v>1</v>
+      </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="8">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R19" s="10"/>
     </row>
@@ -1202,10 +1223,13 @@
       <c r="G21" s="3">
         <v>2</v>
       </c>
+      <c r="H21" s="3">
+        <v>1</v>
+      </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="8">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R21" s="10"/>
     </row>

</xml_diff>

<commit_message>
lucrul cu cifrele unui numar
</commit_message>
<xml_diff>
--- a/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
+++ b/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Geoinformatica_Promotia_2025_2028\AlgoritmiSiStructuriDeDate1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9E24B7-4B63-475A-8A5B-29295A50BD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C1A693-0F23-40AD-BF91-1768C755DDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -676,7 +676,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -853,10 +853,13 @@
       <c r="G7" s="3">
         <v>2</v>
       </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R7" s="10"/>
     </row>
@@ -906,12 +909,12 @@
         <v>1</v>
       </c>
       <c r="H9" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="8">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R9" s="10"/>
     </row>
@@ -934,10 +937,13 @@
       <c r="G10" s="3">
         <v>1</v>
       </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R10" s="10"/>
     </row>
@@ -987,12 +993,12 @@
         <v>2</v>
       </c>
       <c r="H12" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="8">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R12" s="10"/>
     </row>
@@ -1113,10 +1119,13 @@
       <c r="G17" s="3">
         <v>2</v>
       </c>
+      <c r="H17" s="3">
+        <v>1</v>
+      </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="8">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R17" s="10"/>
     </row>
@@ -1169,12 +1178,12 @@
         <v>2</v>
       </c>
       <c r="H19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="8">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R19" s="10"/>
     </row>
@@ -1224,12 +1233,12 @@
         <v>2</v>
       </c>
       <c r="H21" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="8">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R21" s="10"/>
     </row>

</xml_diff>

<commit_message>
Exercitii cu parcurgere de vectori
</commit_message>
<xml_diff>
--- a/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
+++ b/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Geoinformatica_Promotia_2025_2028\AlgoritmiSiStructuriDeDate1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA88EF7-B641-4E4C-9F3B-A52077CB62BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5EBB27-F661-45E8-A8D5-8F42EE3BB292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -676,7 +676,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K18" sqref="K18"/>
+      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -833,10 +833,13 @@
       <c r="I6" s="3">
         <v>2</v>
       </c>
+      <c r="J6" s="3">
+        <v>1</v>
+      </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R6" s="10"/>
     </row>
@@ -923,10 +926,13 @@
       <c r="I9" s="3">
         <v>2</v>
       </c>
+      <c r="J9" s="3">
+        <v>1</v>
+      </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="8">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="R9" s="10"/>
     </row>
@@ -1013,10 +1019,13 @@
       <c r="I12" s="3">
         <v>2</v>
       </c>
+      <c r="J12" s="3">
+        <v>1</v>
+      </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="8">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="R12" s="10"/>
     </row>
@@ -1042,10 +1051,13 @@
       <c r="I13" s="3">
         <v>2</v>
       </c>
+      <c r="J13" s="3">
+        <v>1</v>
+      </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="8">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R13" s="10"/>
     </row>
@@ -1172,10 +1184,13 @@
       <c r="H18" s="3">
         <v>1</v>
       </c>
+      <c r="J18" s="3">
+        <v>1</v>
+      </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="8">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R18" s="10"/>
     </row>
@@ -1201,10 +1216,13 @@
       <c r="H19" s="3">
         <v>2</v>
       </c>
+      <c r="J19" s="3">
+        <v>1</v>
+      </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="8">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="R19" s="10"/>
     </row>
@@ -1259,10 +1277,13 @@
       <c r="I21" s="3">
         <v>2</v>
       </c>
+      <c r="J21" s="3">
+        <v>1</v>
+      </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="8">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="R21" s="10"/>
     </row>

</xml_diff>

<commit_message>
lucru cu metode, compararea rezolvarii a doua exercitii precedente cu rezolvarea folosind metode
</commit_message>
<xml_diff>
--- a/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
+++ b/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Geoinformatica_Promotia_2025_2028\AlgoritmiSiStructuriDeDate1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5EBB27-F661-45E8-A8D5-8F42EE3BB292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E27EE67-DEE9-4929-8B22-513ADDEBE2A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Prenume Nume</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Victor Lazăr</t>
+  </si>
+  <si>
+    <t>Cătălina Mădălina Parca</t>
   </si>
 </sst>
 </file>
@@ -676,7 +679,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
+      <selection pane="bottomRight" activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -792,7 +795,7 @@
       </c>
       <c r="P4" s="10"/>
       <c r="Q4" s="8">
-        <f t="shared" ref="Q4:Q52" si="0">SUM(C4:P4)</f>
+        <f>SUM(C4:P4)</f>
         <v>5</v>
       </c>
       <c r="R4" s="10"/>
@@ -806,7 +809,7 @@
       </c>
       <c r="P5" s="10"/>
       <c r="Q5" s="8">
-        <f t="shared" si="0"/>
+        <f>SUM(C5:P5)</f>
         <v>1</v>
       </c>
       <c r="R5" s="10"/>
@@ -834,61 +837,47 @@
         <v>2</v>
       </c>
       <c r="J6" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f>SUM(C6:P6)</f>
+        <v>12</v>
       </c>
       <c r="R6" s="10"/>
     </row>
     <row r="7" spans="2:18">
       <c r="B7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="9">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-      <c r="F7" s="3">
-        <v>1</v>
-      </c>
-      <c r="G7" s="3">
-        <v>2</v>
-      </c>
-      <c r="H7" s="3">
-        <v>1</v>
-      </c>
-      <c r="I7" s="3">
-        <v>2</v>
+        <v>36</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="J7" s="3">
+        <v>1</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <f>SUM(C7:P7)</f>
+        <v>1</v>
       </c>
       <c r="R7" s="10"/>
     </row>
     <row r="8" spans="2:18">
       <c r="B8" s="4" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C8" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
       </c>
-      <c r="E8" s="3">
-        <v>2</v>
-      </c>
       <c r="F8" s="3">
         <v>1</v>
       </c>
       <c r="G8" s="3">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3">
         <v>1</v>
       </c>
       <c r="I8" s="3">
@@ -896,55 +885,49 @@
       </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="8">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f>SUM(C8:P8)</f>
+        <v>9</v>
       </c>
       <c r="R8" s="10"/>
     </row>
     <row r="9" spans="2:18">
       <c r="B9" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C9" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="3">
         <v>1</v>
       </c>
-      <c r="H9" s="3">
-        <v>2</v>
-      </c>
       <c r="I9" s="3">
         <v>2</v>
-      </c>
-      <c r="J9" s="3">
-        <v>1</v>
       </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="8">
-        <f t="shared" si="0"/>
-        <v>13</v>
+        <f>SUM(C9:P9)</f>
+        <v>8</v>
       </c>
       <c r="R9" s="10"/>
     </row>
     <row r="10" spans="2:18">
       <c r="B10" s="4" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C10" s="9">
         <v>2</v>
       </c>
       <c r="D10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
@@ -956,24 +939,27 @@
         <v>1</v>
       </c>
       <c r="H10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I10" s="3">
         <v>2</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1</v>
       </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="8">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>SUM(C10:P10)</f>
+        <v>13</v>
       </c>
       <c r="R10" s="10"/>
     </row>
     <row r="11" spans="2:18">
       <c r="B11" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C11" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="3">
         <v>1</v>
@@ -982,59 +968,59 @@
         <v>1</v>
       </c>
       <c r="F11" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" s="3">
         <v>1</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3">
+        <v>2</v>
       </c>
       <c r="P11" s="10"/>
       <c r="Q11" s="8">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>SUM(C11:P11)</f>
+        <v>10</v>
       </c>
       <c r="R11" s="10"/>
     </row>
     <row r="12" spans="2:18">
       <c r="B12" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C12" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12" s="3">
-        <v>2</v>
-      </c>
-      <c r="H12" s="3">
-        <v>2</v>
-      </c>
-      <c r="I12" s="3">
-        <v>2</v>
-      </c>
-      <c r="J12" s="3">
         <v>1</v>
       </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="8">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <f>SUM(C12:P12)</f>
+        <v>5</v>
       </c>
       <c r="R12" s="10"/>
     </row>
     <row r="13" spans="2:18">
       <c r="B13" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C13" s="9">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2</v>
       </c>
       <c r="E13" s="3">
         <v>2</v>
@@ -1046,30 +1032,27 @@
         <v>2</v>
       </c>
       <c r="H13" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" s="3">
         <v>2</v>
       </c>
       <c r="J13" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="8">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f>SUM(C13:P13)</f>
+        <v>16</v>
       </c>
       <c r="R13" s="10"/>
     </row>
     <row r="14" spans="2:18">
       <c r="B14" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C14" s="9">
-        <v>2</v>
-      </c>
-      <c r="D14" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" s="3">
         <v>2</v>
@@ -1082,92 +1065,98 @@
       </c>
       <c r="H14" s="3">
         <v>1</v>
+      </c>
+      <c r="I14" s="3">
+        <v>2</v>
+      </c>
+      <c r="J14" s="3">
+        <v>2</v>
       </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="8">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <f>SUM(C14:P14)</f>
+        <v>12</v>
       </c>
       <c r="R14" s="10"/>
     </row>
     <row r="15" spans="2:18">
       <c r="B15" s="4" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C15" s="9">
         <v>2</v>
       </c>
       <c r="D15" s="3">
+        <v>2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3">
+        <v>2</v>
+      </c>
+      <c r="G15" s="3">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3">
         <v>1</v>
       </c>
       <c r="P15" s="10"/>
       <c r="Q15" s="8">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>SUM(C15:P15)</f>
+        <v>11</v>
       </c>
       <c r="R15" s="10"/>
     </row>
     <row r="16" spans="2:18">
       <c r="B16" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" s="9">
         <v>2</v>
       </c>
       <c r="D16" s="3">
-        <v>1</v>
-      </c>
-      <c r="E16" s="3">
-        <v>1</v>
-      </c>
-      <c r="F16" s="3">
-        <v>1</v>
-      </c>
-      <c r="G16" s="3">
         <v>1</v>
       </c>
       <c r="P16" s="10"/>
       <c r="Q16" s="8">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>SUM(C16:P16)</f>
+        <v>3</v>
       </c>
       <c r="R16" s="10"/>
     </row>
     <row r="17" spans="2:18">
       <c r="B17" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C17" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17" s="3">
-        <v>2</v>
-      </c>
-      <c r="H17" s="3">
         <v>1</v>
       </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="8">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>SUM(C17:P17)</f>
+        <v>6</v>
       </c>
       <c r="R17" s="10"/>
     </row>
     <row r="18" spans="2:18">
       <c r="B18" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C18" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="3">
         <v>2</v>
@@ -1182,21 +1171,18 @@
         <v>2</v>
       </c>
       <c r="H18" s="3">
-        <v>1</v>
-      </c>
-      <c r="J18" s="3">
         <v>1</v>
       </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="8">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <f>SUM(C18:P18)</f>
+        <v>10</v>
       </c>
       <c r="R18" s="10"/>
     </row>
     <row r="19" spans="2:18">
       <c r="B19" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C19" s="9">
         <v>2</v>
@@ -1214,86 +1200,108 @@
         <v>2</v>
       </c>
       <c r="H19" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J19" s="3">
         <v>1</v>
       </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="8">
-        <f t="shared" si="0"/>
-        <v>13</v>
+        <f>SUM(C19:P19)</f>
+        <v>12</v>
       </c>
       <c r="R19" s="10"/>
     </row>
     <row r="20" spans="2:18">
       <c r="B20" s="4" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C20" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G20" s="3">
+        <v>2</v>
+      </c>
+      <c r="H20" s="3">
+        <v>2</v>
+      </c>
+      <c r="J20" s="3">
         <v>1</v>
       </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="8">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>SUM(C20:P20)</f>
+        <v>13</v>
       </c>
       <c r="R20" s="10"/>
     </row>
     <row r="21" spans="2:18">
       <c r="B21" s="4" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C21" s="9">
         <v>1</v>
       </c>
       <c r="D21" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21" s="3">
-        <v>2</v>
-      </c>
-      <c r="H21" s="3">
-        <v>2</v>
-      </c>
-      <c r="I21" s="3">
-        <v>2</v>
-      </c>
-      <c r="J21" s="3">
         <v>1</v>
       </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="8">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <f>SUM(C21:P21)</f>
+        <v>5</v>
       </c>
       <c r="R21" s="10"/>
     </row>
     <row r="22" spans="2:18">
-      <c r="B22" s="4"/>
-      <c r="C22" s="9"/>
+      <c r="B22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="9">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3">
+        <v>2</v>
+      </c>
+      <c r="E22" s="3">
+        <v>2</v>
+      </c>
+      <c r="F22" s="3">
+        <v>2</v>
+      </c>
+      <c r="G22" s="3">
+        <v>2</v>
+      </c>
+      <c r="H22" s="3">
+        <v>2</v>
+      </c>
+      <c r="I22" s="3">
+        <v>2</v>
+      </c>
+      <c r="J22" s="3">
+        <v>2</v>
+      </c>
       <c r="P22" s="10"/>
       <c r="Q22" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(C22:P22)</f>
+        <v>15</v>
       </c>
       <c r="R22" s="10"/>
     </row>
@@ -1302,7 +1310,7 @@
       <c r="C23" s="9"/>
       <c r="P23" s="10"/>
       <c r="Q23" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q4:Q52" si="0">SUM(C23:P23)</f>
         <v>0</v>
       </c>
       <c r="R23" s="10"/>
@@ -1610,8 +1618,8 @@
       <c r="R52" s="14"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:R52">
-    <sortCondition ref="B52"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:Q22">
+    <sortCondition ref="B3:B22"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q52">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
desenat bradut in consola
</commit_message>
<xml_diff>
--- a/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
+++ b/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Geoinformatica_Promotia_2025_2028\AlgoritmiSiStructuriDeDate1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E27EE67-DEE9-4929-8B22-513ADDEBE2A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98730F9D-17A5-42AE-BE03-E652595651EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -135,7 +135,7 @@
     <t>Victor Lazăr</t>
   </si>
   <si>
-    <t>Cătălina Mădălina Parca</t>
+    <t>Cătălina Mădălina Paca</t>
   </si>
 </sst>
 </file>
@@ -679,7 +679,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M17" sqref="M17"/>
+      <selection pane="bottomRight" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -769,7 +769,7 @@
       <c r="O3" s="6"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="8">
-        <f>SUM(C3:P3)</f>
+        <f t="shared" ref="Q3:Q22" si="0">SUM(C3:P3)</f>
         <v>8</v>
       </c>
       <c r="R3" s="7"/>
@@ -795,7 +795,7 @@
       </c>
       <c r="P4" s="10"/>
       <c r="Q4" s="8">
-        <f>SUM(C4:P4)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="R4" s="10"/>
@@ -809,7 +809,7 @@
       </c>
       <c r="P5" s="10"/>
       <c r="Q5" s="8">
-        <f>SUM(C5:P5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R5" s="10"/>
@@ -841,7 +841,7 @@
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8">
-        <f>SUM(C6:P6)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="R6" s="10"/>
@@ -854,10 +854,13 @@
       <c r="J7" s="3">
         <v>1</v>
       </c>
+      <c r="K7" s="3">
+        <v>2</v>
+      </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8">
-        <f>SUM(C7:P7)</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R7" s="10"/>
     </row>
@@ -885,7 +888,7 @@
       </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="8">
-        <f>SUM(C8:P8)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="R8" s="10"/>
@@ -914,7 +917,7 @@
       </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="8">
-        <f>SUM(C9:P9)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="R9" s="10"/>
@@ -947,10 +950,13 @@
       <c r="J10" s="3">
         <v>1</v>
       </c>
+      <c r="K10" s="3">
+        <v>2</v>
+      </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="8">
-        <f>SUM(C10:P10)</f>
-        <v>13</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="R10" s="10"/>
     </row>
@@ -981,7 +987,7 @@
       </c>
       <c r="P11" s="10"/>
       <c r="Q11" s="8">
-        <f>SUM(C11:P11)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="R11" s="10"/>
@@ -1007,7 +1013,7 @@
       </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="8">
-        <f>SUM(C12:P12)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="R12" s="10"/>
@@ -1040,10 +1046,13 @@
       <c r="J13" s="3">
         <v>2</v>
       </c>
+      <c r="K13" s="3">
+        <v>2</v>
+      </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="8">
-        <f>SUM(C13:P13)</f>
-        <v>16</v>
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
       <c r="R13" s="10"/>
     </row>
@@ -1074,7 +1083,7 @@
       </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="8">
-        <f>SUM(C14:P14)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="R14" s="10"/>
@@ -1101,10 +1110,13 @@
       <c r="H15" s="3">
         <v>1</v>
       </c>
+      <c r="K15" s="3">
+        <v>2</v>
+      </c>
       <c r="P15" s="10"/>
       <c r="Q15" s="8">
-        <f>SUM(C15:P15)</f>
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
       <c r="R15" s="10"/>
     </row>
@@ -1120,7 +1132,7 @@
       </c>
       <c r="P16" s="10"/>
       <c r="Q16" s="8">
-        <f>SUM(C16:P16)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R16" s="10"/>
@@ -1146,7 +1158,7 @@
       </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="8">
-        <f>SUM(C17:P17)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="R17" s="10"/>
@@ -1175,7 +1187,7 @@
       </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="8">
-        <f>SUM(C18:P18)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="R18" s="10"/>
@@ -1207,7 +1219,7 @@
       </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="8">
-        <f>SUM(C19:P19)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="R19" s="10"/>
@@ -1237,10 +1249,13 @@
       <c r="J20" s="3">
         <v>1</v>
       </c>
+      <c r="K20" s="3">
+        <v>2</v>
+      </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="8">
-        <f>SUM(C20:P20)</f>
-        <v>13</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="R20" s="10"/>
     </row>
@@ -1265,7 +1280,7 @@
       </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="8">
-        <f>SUM(C21:P21)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="R21" s="10"/>
@@ -1298,10 +1313,13 @@
       <c r="J22" s="3">
         <v>2</v>
       </c>
+      <c r="K22" s="3">
+        <v>2</v>
+      </c>
       <c r="P22" s="10"/>
       <c r="Q22" s="8">
-        <f>SUM(C22:P22)</f>
-        <v>15</v>
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
       <c r="R22" s="10"/>
     </row>
@@ -1310,7 +1328,7 @@
       <c r="C23" s="9"/>
       <c r="P23" s="10"/>
       <c r="Q23" s="8">
-        <f t="shared" ref="Q4:Q52" si="0">SUM(C23:P23)</f>
+        <f t="shared" ref="Q23:Q52" si="1">SUM(C23:P23)</f>
         <v>0</v>
       </c>
       <c r="R23" s="10"/>
@@ -1320,7 +1338,7 @@
       <c r="C24" s="9"/>
       <c r="P24" s="10"/>
       <c r="Q24" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R24" s="10"/>
@@ -1330,7 +1348,7 @@
       <c r="C25" s="9"/>
       <c r="P25" s="10"/>
       <c r="Q25" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R25" s="10"/>
@@ -1340,7 +1358,7 @@
       <c r="C26" s="9"/>
       <c r="P26" s="10"/>
       <c r="Q26" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R26" s="10"/>
@@ -1350,7 +1368,7 @@
       <c r="C27" s="9"/>
       <c r="P27" s="10"/>
       <c r="Q27" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R27" s="10"/>
@@ -1360,7 +1378,7 @@
       <c r="C28" s="9"/>
       <c r="P28" s="10"/>
       <c r="Q28" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R28" s="10"/>
@@ -1370,7 +1388,7 @@
       <c r="C29" s="9"/>
       <c r="P29" s="10"/>
       <c r="Q29" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R29" s="10"/>
@@ -1380,7 +1398,7 @@
       <c r="C30" s="9"/>
       <c r="P30" s="10"/>
       <c r="Q30" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R30" s="10"/>
@@ -1390,7 +1408,7 @@
       <c r="C31" s="9"/>
       <c r="P31" s="10"/>
       <c r="Q31" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R31" s="10"/>
@@ -1400,7 +1418,7 @@
       <c r="C32" s="9"/>
       <c r="P32" s="10"/>
       <c r="Q32" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R32" s="10"/>
@@ -1410,7 +1428,7 @@
       <c r="C33" s="9"/>
       <c r="P33" s="10"/>
       <c r="Q33" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R33" s="10"/>
@@ -1420,7 +1438,7 @@
       <c r="C34" s="9"/>
       <c r="P34" s="10"/>
       <c r="Q34" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R34" s="10"/>
@@ -1430,7 +1448,7 @@
       <c r="C35" s="9"/>
       <c r="P35" s="10"/>
       <c r="Q35" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R35" s="10"/>
@@ -1440,7 +1458,7 @@
       <c r="C36" s="9"/>
       <c r="P36" s="10"/>
       <c r="Q36" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R36" s="10"/>
@@ -1450,7 +1468,7 @@
       <c r="C37" s="9"/>
       <c r="P37" s="10"/>
       <c r="Q37" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R37" s="10"/>
@@ -1460,7 +1478,7 @@
       <c r="C38" s="9"/>
       <c r="P38" s="10"/>
       <c r="Q38" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R38" s="10"/>
@@ -1470,7 +1488,7 @@
       <c r="C39" s="9"/>
       <c r="P39" s="10"/>
       <c r="Q39" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R39" s="10"/>
@@ -1480,7 +1498,7 @@
       <c r="C40" s="9"/>
       <c r="P40" s="10"/>
       <c r="Q40" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R40" s="10"/>
@@ -1490,7 +1508,7 @@
       <c r="C41" s="9"/>
       <c r="P41" s="10"/>
       <c r="Q41" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R41" s="10"/>
@@ -1500,7 +1518,7 @@
       <c r="C42" s="9"/>
       <c r="P42" s="10"/>
       <c r="Q42" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R42" s="10"/>
@@ -1510,7 +1528,7 @@
       <c r="C43" s="9"/>
       <c r="P43" s="10"/>
       <c r="Q43" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R43" s="10"/>
@@ -1520,7 +1538,7 @@
       <c r="C44" s="9"/>
       <c r="P44" s="10"/>
       <c r="Q44" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R44" s="10"/>
@@ -1530,7 +1548,7 @@
       <c r="C45" s="9"/>
       <c r="P45" s="10"/>
       <c r="Q45" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R45" s="10"/>
@@ -1540,7 +1558,7 @@
       <c r="C46" s="9"/>
       <c r="P46" s="10"/>
       <c r="Q46" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R46" s="10"/>
@@ -1550,7 +1568,7 @@
       <c r="C47" s="9"/>
       <c r="P47" s="10"/>
       <c r="Q47" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R47" s="10"/>
@@ -1560,7 +1578,7 @@
       <c r="C48" s="9"/>
       <c r="P48" s="10"/>
       <c r="Q48" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R48" s="10"/>
@@ -1570,7 +1588,7 @@
       <c r="C49" s="9"/>
       <c r="P49" s="10"/>
       <c r="Q49" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R49" s="10"/>
@@ -1580,7 +1598,7 @@
       <c r="C50" s="9"/>
       <c r="P50" s="10"/>
       <c r="Q50" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R50" s="10"/>
@@ -1590,7 +1608,7 @@
       <c r="C51" s="9"/>
       <c r="P51" s="10"/>
       <c r="Q51" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R51" s="10"/>
@@ -1612,7 +1630,7 @@
       <c r="O52" s="13"/>
       <c r="P52" s="14"/>
       <c r="Q52" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R52" s="14"/>

</xml_diff>

<commit_message>
foreach si structuri repetitive
</commit_message>
<xml_diff>
--- a/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
+++ b/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Geoinformatica_Promotia_2025_2028\AlgoritmiSiStructuriDeDate1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98730F9D-17A5-42AE-BE03-E652595651EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1BA8C7-C719-442A-8CDF-3682CE885115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -679,7 +679,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M12" sqref="M12"/>
+      <selection pane="bottomRight" activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -833,16 +833,19 @@
       <c r="H6" s="3">
         <v>1</v>
       </c>
-      <c r="I6" s="3">
-        <v>2</v>
-      </c>
       <c r="J6" s="3">
         <v>2</v>
+      </c>
+      <c r="K6" s="3">
+        <v>2</v>
+      </c>
+      <c r="M6" s="3">
+        <v>1</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="R6" s="10"/>
     </row>
@@ -851,16 +854,19 @@
         <v>36</v>
       </c>
       <c r="C7" s="9"/>
-      <c r="J7" s="3">
-        <v>1</v>
-      </c>
       <c r="K7" s="3">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="L7" s="3">
+        <v>2</v>
+      </c>
+      <c r="M7" s="3">
+        <v>1</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R7" s="10"/>
     </row>
@@ -883,13 +889,16 @@
       <c r="H8" s="3">
         <v>1</v>
       </c>
-      <c r="I8" s="3">
-        <v>2</v>
+      <c r="J8" s="3">
+        <v>2</v>
+      </c>
+      <c r="M8" s="3">
+        <v>1</v>
       </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="8">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R8" s="10"/>
     </row>
@@ -912,7 +921,7 @@
       <c r="G9" s="3">
         <v>1</v>
       </c>
-      <c r="I9" s="3">
+      <c r="J9" s="3">
         <v>2</v>
       </c>
       <c r="P9" s="10"/>
@@ -944,19 +953,22 @@
       <c r="H10" s="3">
         <v>2</v>
       </c>
-      <c r="I10" s="3">
-        <v>2</v>
-      </c>
       <c r="J10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K10" s="3">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="L10" s="3">
+        <v>2</v>
+      </c>
+      <c r="M10" s="3">
+        <v>1</v>
       </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="8">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R10" s="10"/>
     </row>
@@ -982,7 +994,7 @@
       <c r="H11" s="3">
         <v>1</v>
       </c>
-      <c r="I11" s="3">
+      <c r="J11" s="3">
         <v>2</v>
       </c>
       <c r="P11" s="10"/>
@@ -1040,19 +1052,22 @@
       <c r="H13" s="3">
         <v>2</v>
       </c>
-      <c r="I13" s="3">
-        <v>2</v>
-      </c>
       <c r="J13" s="3">
         <v>2</v>
       </c>
       <c r="K13" s="3">
         <v>2</v>
+      </c>
+      <c r="L13" s="3">
+        <v>2</v>
+      </c>
+      <c r="M13" s="3">
+        <v>1</v>
       </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="8">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R13" s="10"/>
     </row>
@@ -1075,16 +1090,19 @@
       <c r="H14" s="3">
         <v>1</v>
       </c>
-      <c r="I14" s="3">
-        <v>2</v>
-      </c>
       <c r="J14" s="3">
         <v>2</v>
+      </c>
+      <c r="K14" s="3">
+        <v>2</v>
+      </c>
+      <c r="M14" s="3">
+        <v>1</v>
       </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="8">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="R14" s="10"/>
     </row>
@@ -1110,13 +1128,16 @@
       <c r="H15" s="3">
         <v>1</v>
       </c>
-      <c r="K15" s="3">
-        <v>2</v>
+      <c r="L15" s="3">
+        <v>2</v>
+      </c>
+      <c r="M15" s="3">
+        <v>1</v>
       </c>
       <c r="P15" s="10"/>
       <c r="Q15" s="8">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="R15" s="10"/>
     </row>
@@ -1214,7 +1235,7 @@
       <c r="H19" s="3">
         <v>1</v>
       </c>
-      <c r="J19" s="3">
+      <c r="K19" s="3">
         <v>1</v>
       </c>
       <c r="P19" s="10"/>
@@ -1246,16 +1267,19 @@
       <c r="H20" s="3">
         <v>2</v>
       </c>
-      <c r="J20" s="3">
-        <v>1</v>
-      </c>
       <c r="K20" s="3">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="L20" s="3">
+        <v>2</v>
+      </c>
+      <c r="M20" s="3">
+        <v>1</v>
       </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="8">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R20" s="10"/>
     </row>
@@ -1307,19 +1331,22 @@
       <c r="H22" s="3">
         <v>2</v>
       </c>
-      <c r="I22" s="3">
-        <v>2</v>
-      </c>
       <c r="J22" s="3">
         <v>2</v>
       </c>
       <c r="K22" s="3">
         <v>2</v>
+      </c>
+      <c r="L22" s="3">
+        <v>2</v>
+      </c>
+      <c r="M22" s="3">
+        <v>1</v>
       </c>
       <c r="P22" s="10"/>
       <c r="Q22" s="8">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R22" s="10"/>
     </row>

</xml_diff>

<commit_message>
diferite exercitii cu verificarea ordonarii vectorului
</commit_message>
<xml_diff>
--- a/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
+++ b/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Geoinformatica_Promotia_2025_2028\AlgoritmiSiStructuriDeDate1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1EFA59-78F0-4CD5-A3CB-CCDBDF561C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BB9FFA-84BB-460E-967F-BE79A4A34728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -679,7 +679,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
+      <selection pane="bottomRight" activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -793,10 +793,13 @@
       <c r="G4" s="3">
         <v>1</v>
       </c>
+      <c r="N4" s="3">
+        <v>2</v>
+      </c>
       <c r="P4" s="10"/>
       <c r="Q4" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="R4" s="10"/>
     </row>
@@ -863,10 +866,13 @@
       <c r="M7" s="3">
         <v>2</v>
       </c>
+      <c r="N7" s="3">
+        <v>2</v>
+      </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="R7" s="10"/>
     </row>
@@ -965,10 +971,13 @@
       <c r="M10" s="3">
         <v>2</v>
       </c>
+      <c r="N10" s="3">
+        <v>2</v>
+      </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="8">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="R10" s="10"/>
     </row>
@@ -1023,10 +1032,13 @@
       <c r="G12" s="3">
         <v>1</v>
       </c>
+      <c r="N12" s="3">
+        <v>2</v>
+      </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="R12" s="10"/>
     </row>
@@ -1064,10 +1076,13 @@
       <c r="M13" s="3">
         <v>2</v>
       </c>
+      <c r="N13" s="3">
+        <v>2</v>
+      </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="8">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="R13" s="10"/>
     </row>
@@ -1276,10 +1291,13 @@
       <c r="M20" s="3">
         <v>2</v>
       </c>
+      <c r="N20" s="3">
+        <v>2</v>
+      </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="8">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="R20" s="10"/>
     </row>
@@ -1343,10 +1361,13 @@
       <c r="M22" s="3">
         <v>2</v>
       </c>
+      <c r="N22" s="3">
+        <v>2</v>
+      </c>
       <c r="P22" s="10"/>
       <c r="Q22" s="8">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="R22" s="10"/>
     </row>

</xml_diff>

<commit_message>
note algoritmi + fisiere intrebari examen
</commit_message>
<xml_diff>
--- a/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
+++ b/AlgoritmiSiStructuriDeDate1/Prezenta Algoritmi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Geoinformatica_Promotia_2025_2028\AlgoritmiSiStructuriDeDate1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BB9FFA-84BB-460E-967F-BE79A4A34728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576168EA-084C-4EC5-AC9E-62B55B8A1B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -679,7 +679,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M21" sqref="M21"/>
+      <selection pane="bottomRight" activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -767,10 +767,12 @@
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
-      <c r="P3" s="7"/>
+      <c r="P3" s="7">
+        <v>1</v>
+      </c>
       <c r="Q3" s="8">
         <f t="shared" ref="Q3:Q22" si="0">SUM(C3:P3)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R3" s="7"/>
     </row>
@@ -796,10 +798,12 @@
       <c r="N4" s="3">
         <v>2</v>
       </c>
-      <c r="P4" s="10"/>
+      <c r="P4" s="10">
+        <v>1</v>
+      </c>
       <c r="Q4" s="8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R4" s="10"/>
     </row>
@@ -845,10 +849,12 @@
       <c r="M6" s="3">
         <v>1</v>
       </c>
-      <c r="P6" s="10"/>
+      <c r="P6" s="10">
+        <v>1</v>
+      </c>
       <c r="Q6" s="8">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="R6" s="10"/>
     </row>
@@ -901,10 +907,12 @@
       <c r="M8" s="3">
         <v>2</v>
       </c>
-      <c r="P8" s="10"/>
+      <c r="P8" s="10">
+        <v>1</v>
+      </c>
       <c r="Q8" s="8">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R8" s="10"/>
     </row>
@@ -974,10 +982,12 @@
       <c r="N10" s="3">
         <v>2</v>
       </c>
-      <c r="P10" s="10"/>
+      <c r="P10" s="10">
+        <v>1</v>
+      </c>
       <c r="Q10" s="8">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R10" s="10"/>
     </row>
@@ -1006,10 +1016,12 @@
       <c r="J11" s="3">
         <v>2</v>
       </c>
-      <c r="P11" s="10"/>
+      <c r="P11" s="10">
+        <v>1</v>
+      </c>
       <c r="Q11" s="8">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R11" s="10"/>
     </row>
@@ -1035,10 +1047,12 @@
       <c r="N12" s="3">
         <v>2</v>
       </c>
-      <c r="P12" s="10"/>
+      <c r="P12" s="10">
+        <v>1</v>
+      </c>
       <c r="Q12" s="8">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R12" s="10"/>
     </row>
@@ -1079,10 +1093,12 @@
       <c r="N13" s="3">
         <v>2</v>
       </c>
-      <c r="P13" s="10"/>
+      <c r="P13" s="10">
+        <v>1</v>
+      </c>
       <c r="Q13" s="8">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R13" s="10"/>
     </row>
@@ -1114,10 +1130,12 @@
       <c r="M14" s="3">
         <v>1</v>
       </c>
-      <c r="P14" s="10"/>
+      <c r="P14" s="10">
+        <v>1</v>
+      </c>
       <c r="Q14" s="8">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="R14" s="10"/>
     </row>
@@ -1149,10 +1167,12 @@
       <c r="M15" s="3">
         <v>2</v>
       </c>
-      <c r="P15" s="10"/>
+      <c r="P15" s="10">
+        <v>1</v>
+      </c>
       <c r="Q15" s="8">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R15" s="10"/>
     </row>
@@ -1192,10 +1212,12 @@
       <c r="G17" s="3">
         <v>1</v>
       </c>
-      <c r="P17" s="10"/>
+      <c r="P17" s="10">
+        <v>1</v>
+      </c>
       <c r="Q17" s="8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R17" s="10"/>
     </row>
@@ -1221,10 +1243,12 @@
       <c r="H18" s="3">
         <v>1</v>
       </c>
-      <c r="P18" s="10"/>
+      <c r="P18" s="10">
+        <v>1</v>
+      </c>
       <c r="Q18" s="8">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R18" s="10"/>
     </row>
@@ -1253,10 +1277,12 @@
       <c r="K19" s="3">
         <v>1</v>
       </c>
-      <c r="P19" s="10"/>
+      <c r="P19" s="10">
+        <v>1</v>
+      </c>
       <c r="Q19" s="8">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="R19" s="10"/>
     </row>
@@ -1294,10 +1320,12 @@
       <c r="N20" s="3">
         <v>2</v>
       </c>
-      <c r="P20" s="10"/>
+      <c r="P20" s="10">
+        <v>1</v>
+      </c>
       <c r="Q20" s="8">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R20" s="10"/>
     </row>
@@ -1364,10 +1392,12 @@
       <c r="N22" s="3">
         <v>2</v>
       </c>
-      <c r="P22" s="10"/>
+      <c r="P22" s="10">
+        <v>1</v>
+      </c>
       <c r="Q22" s="8">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="R22" s="10"/>
     </row>

</xml_diff>